<commit_message>
All Country Files Saved And Formatted
</commit_message>
<xml_diff>
--- a/Datasets/SeperateCountryFiles/Angola.xlsx
+++ b/Datasets/SeperateCountryFiles/Angola.xlsx
@@ -16,8 +16,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="yyyy-mm-dd;"/>
   </numFmts>
   <fonts count="1">
     <font>
@@ -48,9 +49,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -348,417 +355,565 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L10"/>
+  <dimension ref="A1:O11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <cols>
+    <col width="27" customWidth="1" min="1" max="1"/>
+    <col width="27" customWidth="1" min="2" max="2"/>
+    <col width="27" customWidth="1" min="3" max="3"/>
+    <col width="27" customWidth="1" min="4" max="4"/>
+    <col width="27" customWidth="1" min="5" max="5"/>
+    <col width="27" customWidth="1" min="6" max="6"/>
+    <col width="27" customWidth="1" min="7" max="7"/>
+    <col width="27" customWidth="1" min="8" max="8"/>
+    <col width="27" customWidth="1" min="9" max="9"/>
+    <col width="27" customWidth="1" min="10" max="10"/>
+    <col width="27" customWidth="1" min="11" max="11"/>
+    <col width="27" customWidth="1" min="12" max="12"/>
+    <col width="27" customWidth="1" min="13" max="13"/>
+    <col width="27" customWidth="1" min="14" max="14"/>
+    <col width="27" customWidth="1" min="15" max="15"/>
+  </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
+      <c r="A1" s="2" t="inlineStr">
         <is>
           <t>No Of Sit_Rep</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="B1" s="2" t="inlineStr">
         <is>
           <t>CountryID</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="C1" s="2" t="inlineStr">
         <is>
           <t>WorldRegion</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="D1" s="3" t="inlineStr">
         <is>
           <t>Date</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="E1" s="2" t="inlineStr">
         <is>
           <t>CountryName</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="F1" s="2" t="inlineStr">
         <is>
           <t>TotalConfirmedCases</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="G1" s="2" t="inlineStr">
         <is>
           <t>TotalConfirmedNewCases</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="H1" s="2" t="inlineStr">
         <is>
           <t>TotalDeaths</t>
         </is>
       </c>
-      <c r="I1" t="inlineStr">
+      <c r="I1" s="2" t="inlineStr">
         <is>
           <t>TotalNewDeaths</t>
         </is>
       </c>
-      <c r="J1" t="inlineStr">
+      <c r="J1" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve">TransmissionClassification </t>
         </is>
       </c>
-      <c r="K1" t="inlineStr">
+      <c r="K1" s="2" t="inlineStr">
         <is>
           <t>DaysSinceLastReportedCase</t>
         </is>
       </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>RowNo.</t>
-        </is>
-      </c>
+      <c r="L1" s="2" t="inlineStr">
+        <is>
+          <t>MasterSheet RowNo.</t>
+        </is>
+      </c>
+      <c r="M1" s="2" t="n"/>
+      <c r="N1" s="2" t="n"/>
+      <c r="O1" s="2" t="n"/>
     </row>
     <row r="2">
-      <c r="A2" t="n">
+      <c r="A2" s="2" t="n">
         <v>62</v>
       </c>
-      <c r="B2" t="n">
-        <v>6</v>
-      </c>
-      <c r="C2" t="inlineStr">
+      <c r="B2" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="C2" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve">SUB-SAHARAN AFRICA                 </t>
         </is>
       </c>
-      <c r="D2" s="1" t="n">
+      <c r="D2" s="3" t="n">
         <v>43912</v>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="E2" s="2" t="inlineStr">
         <is>
           <t>Angola</t>
         </is>
       </c>
-      <c r="F2" t="n">
-        <v>2</v>
-      </c>
-      <c r="H2" t="n">
-        <v>0</v>
-      </c>
-      <c r="J2" t="inlineStr">
+      <c r="F2" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="G2" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="H2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J2" s="2" t="inlineStr">
         <is>
           <t>Imported cases only</t>
         </is>
       </c>
-      <c r="K2" t="n">
-        <v>0</v>
-      </c>
-      <c r="L2" t="n">
+      <c r="K2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L2" s="2" t="n">
         <v>3628</v>
       </c>
+      <c r="M2" s="2" t="n"/>
+      <c r="N2" s="2" t="n"/>
+      <c r="O2" s="2" t="n"/>
     </row>
     <row r="3">
-      <c r="A3" t="n">
+      <c r="A3" s="2" t="n">
         <v>63</v>
       </c>
-      <c r="B3" t="n">
-        <v>6</v>
-      </c>
-      <c r="C3" t="inlineStr">
+      <c r="B3" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="C3" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve">SUB-SAHARAN AFRICA                 </t>
         </is>
       </c>
-      <c r="D3" s="1" t="n">
+      <c r="D3" s="3" t="n">
         <v>43913</v>
       </c>
-      <c r="E3" t="inlineStr">
+      <c r="E3" s="2" t="inlineStr">
         <is>
           <t>Angola</t>
         </is>
       </c>
-      <c r="F3" t="n">
-        <v>2</v>
-      </c>
-      <c r="H3" t="n">
-        <v>0</v>
-      </c>
-      <c r="J3" t="inlineStr">
+      <c r="F3" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="G3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J3" s="2" t="inlineStr">
         <is>
           <t>Imported cases only</t>
         </is>
       </c>
-      <c r="K3" t="n">
+      <c r="K3" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="L3" t="n">
+      <c r="L3" s="2" t="n">
         <v>3820</v>
       </c>
+      <c r="M3" s="2" t="n"/>
+      <c r="N3" s="2" t="n"/>
+      <c r="O3" s="2" t="n"/>
     </row>
     <row r="4">
-      <c r="A4" t="n">
+      <c r="A4" s="2" t="n">
         <v>64</v>
       </c>
-      <c r="B4" t="n">
-        <v>6</v>
-      </c>
-      <c r="C4" t="inlineStr">
+      <c r="B4" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="C4" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve">SUB-SAHARAN AFRICA                 </t>
         </is>
       </c>
-      <c r="D4" s="1" t="n">
+      <c r="D4" s="3" t="n">
         <v>43914</v>
       </c>
-      <c r="E4" t="inlineStr">
+      <c r="E4" s="2" t="inlineStr">
         <is>
           <t>Angola</t>
         </is>
       </c>
-      <c r="F4" t="n">
-        <v>2</v>
-      </c>
-      <c r="H4" t="n">
-        <v>0</v>
-      </c>
-      <c r="J4" t="inlineStr">
+      <c r="F4" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="G4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J4" s="2" t="inlineStr">
         <is>
           <t>Imported cases only</t>
         </is>
       </c>
-      <c r="K4" t="n">
-        <v>2</v>
-      </c>
-      <c r="L4" t="n">
+      <c r="K4" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="L4" s="2" t="n">
         <v>4019</v>
       </c>
+      <c r="M4" s="2" t="n"/>
+      <c r="N4" s="2" t="n"/>
+      <c r="O4" s="2" t="n"/>
     </row>
     <row r="5">
-      <c r="A5" t="n">
+      <c r="A5" s="2" t="n">
         <v>65</v>
       </c>
-      <c r="B5" t="n">
-        <v>6</v>
-      </c>
-      <c r="C5" t="inlineStr">
+      <c r="B5" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="C5" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve">SUB-SAHARAN AFRICA                 </t>
         </is>
       </c>
-      <c r="D5" s="1" t="n">
+      <c r="D5" s="3" t="n">
         <v>43915</v>
       </c>
-      <c r="E5" t="inlineStr">
+      <c r="E5" s="2" t="inlineStr">
         <is>
           <t>Angola</t>
         </is>
       </c>
-      <c r="F5" t="n">
-        <v>2</v>
-      </c>
-      <c r="H5" t="n">
-        <v>0</v>
-      </c>
-      <c r="J5" t="inlineStr">
+      <c r="F5" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="G5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J5" s="2" t="inlineStr">
         <is>
           <t>Imported cases only</t>
         </is>
       </c>
-      <c r="K5" t="n">
+      <c r="K5" s="2" t="n">
         <v>3</v>
       </c>
-      <c r="L5" t="n">
+      <c r="L5" s="2" t="n">
         <v>4217</v>
       </c>
+      <c r="M5" s="2" t="n"/>
+      <c r="N5" s="2" t="n"/>
+      <c r="O5" s="2" t="n"/>
     </row>
     <row r="6">
-      <c r="A6" t="n">
+      <c r="A6" s="2" t="n">
         <v>66</v>
       </c>
-      <c r="B6" t="n">
-        <v>6</v>
-      </c>
-      <c r="C6" t="inlineStr">
+      <c r="B6" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="C6" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve">SUB-SAHARAN AFRICA                 </t>
         </is>
       </c>
-      <c r="D6" s="1" t="n">
+      <c r="D6" s="3" t="n">
         <v>43916</v>
       </c>
-      <c r="E6" t="inlineStr">
+      <c r="E6" s="2" t="inlineStr">
         <is>
           <t>Angola</t>
         </is>
       </c>
-      <c r="F6" t="n">
-        <v>2</v>
-      </c>
-      <c r="H6" t="n">
-        <v>0</v>
-      </c>
-      <c r="J6" t="inlineStr">
+      <c r="F6" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="G6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J6" s="2" t="inlineStr">
         <is>
           <t>Imported cases only</t>
         </is>
       </c>
-      <c r="K6" t="n">
+      <c r="K6" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="L6" t="n">
+      <c r="L6" s="2" t="n">
         <v>4413</v>
       </c>
+      <c r="M6" s="2" t="n"/>
+      <c r="N6" s="2" t="n"/>
+      <c r="O6" s="2" t="n"/>
     </row>
     <row r="7">
-      <c r="A7" t="n">
+      <c r="A7" s="2" t="n">
         <v>67</v>
       </c>
-      <c r="B7" t="n">
-        <v>6</v>
-      </c>
-      <c r="C7" t="inlineStr">
+      <c r="B7" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="C7" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve">SUB-SAHARAN AFRICA                 </t>
         </is>
       </c>
-      <c r="D7" s="1" t="n">
+      <c r="D7" s="3" t="n">
         <v>43917</v>
       </c>
-      <c r="E7" t="inlineStr">
+      <c r="E7" s="2" t="inlineStr">
         <is>
           <t>Angola</t>
         </is>
       </c>
-      <c r="F7" t="n">
-        <v>2</v>
-      </c>
-      <c r="H7" t="n">
-        <v>0</v>
-      </c>
-      <c r="J7" t="inlineStr">
+      <c r="F7" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="G7" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I7" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J7" s="2" t="inlineStr">
         <is>
           <t>Imported cases only</t>
         </is>
       </c>
-      <c r="K7" t="n">
+      <c r="K7" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="L7" t="n">
+      <c r="L7" s="2" t="n">
         <v>4614</v>
       </c>
+      <c r="M7" s="2" t="n"/>
+      <c r="N7" s="2" t="n"/>
+      <c r="O7" s="2" t="n"/>
     </row>
     <row r="8">
-      <c r="A8" t="n">
+      <c r="A8" s="2" t="n">
         <v>68</v>
       </c>
-      <c r="B8" t="n">
-        <v>6</v>
-      </c>
-      <c r="C8" t="inlineStr">
+      <c r="B8" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="C8" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve">SUB-SAHARAN AFRICA                 </t>
         </is>
       </c>
-      <c r="D8" s="1" t="n">
+      <c r="D8" s="3" t="n">
         <v>43918</v>
       </c>
-      <c r="E8" t="inlineStr">
+      <c r="E8" s="2" t="inlineStr">
         <is>
           <t>Angola</t>
         </is>
       </c>
-      <c r="F8" t="n">
-        <v>2</v>
-      </c>
-      <c r="H8" t="n">
-        <v>0</v>
-      </c>
-      <c r="J8" t="inlineStr">
+      <c r="F8" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="G8" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H8" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I8" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J8" s="2" t="inlineStr">
         <is>
           <t>Imported cases only</t>
         </is>
       </c>
-      <c r="K8" t="n">
-        <v>6</v>
-      </c>
-      <c r="L8" t="n">
+      <c r="K8" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="L8" s="2" t="n">
         <v>4813</v>
       </c>
+      <c r="M8" s="2" t="n"/>
+      <c r="N8" s="2" t="n"/>
+      <c r="O8" s="2" t="n"/>
     </row>
     <row r="9">
-      <c r="A9" t="n">
+      <c r="A9" s="2" t="n">
         <v>69</v>
       </c>
-      <c r="B9" t="n">
-        <v>6</v>
-      </c>
-      <c r="C9" t="inlineStr">
+      <c r="B9" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="C9" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve">SUB-SAHARAN AFRICA                 </t>
         </is>
       </c>
-      <c r="D9" s="1" t="n">
+      <c r="D9" s="3" t="n">
         <v>43919</v>
       </c>
-      <c r="E9" t="inlineStr">
+      <c r="E9" s="2" t="inlineStr">
         <is>
           <t>Angola</t>
         </is>
       </c>
-      <c r="F9" t="n">
-        <v>2</v>
-      </c>
-      <c r="H9" t="n">
-        <v>0</v>
-      </c>
-      <c r="J9" t="inlineStr">
+      <c r="F9" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="G9" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H9" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I9" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J9" s="2" t="inlineStr">
         <is>
           <t>Imported cases only</t>
         </is>
       </c>
-      <c r="K9" t="n">
+      <c r="K9" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="L9" t="n">
+      <c r="L9" s="2" t="n">
         <v>5017</v>
       </c>
+      <c r="M9" s="2" t="n"/>
+      <c r="N9" s="2" t="n"/>
+      <c r="O9" s="2" t="n"/>
     </row>
     <row r="10">
-      <c r="A10" t="n">
+      <c r="A10" s="2" t="n">
         <v>70</v>
       </c>
-      <c r="B10" t="n">
-        <v>6</v>
-      </c>
-      <c r="C10" t="inlineStr">
+      <c r="B10" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="C10" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve">SUB-SAHARAN AFRICA                 </t>
         </is>
       </c>
-      <c r="D10" s="1" t="n">
+      <c r="D10" s="3" t="n">
         <v>43920</v>
       </c>
-      <c r="E10" t="inlineStr">
+      <c r="E10" s="2" t="inlineStr">
         <is>
           <t>Angola</t>
         </is>
       </c>
-      <c r="F10" t="n">
-        <v>2</v>
-      </c>
-      <c r="H10" t="n">
-        <v>0</v>
-      </c>
-      <c r="J10" t="inlineStr">
+      <c r="F10" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="G10" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H10" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I10" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J10" s="2" t="inlineStr">
         <is>
           <t>Imported cases only</t>
         </is>
       </c>
-      <c r="K10" t="n">
+      <c r="K10" s="2" t="n">
         <v>8</v>
       </c>
-      <c r="L10" t="n">
-        <v>5221</v>
-      </c>
+      <c r="L10" s="2" t="n">
+        <v>5220</v>
+      </c>
+      <c r="M10" s="2" t="n"/>
+      <c r="N10" s="2" t="n"/>
+      <c r="O10" s="2" t="n"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="2" t="n">
+        <v>71</v>
+      </c>
+      <c r="B11" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="C11" s="2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">SUB-SAHARAN AFRICA                 </t>
+        </is>
+      </c>
+      <c r="D11" s="3" t="n">
+        <v>43921</v>
+      </c>
+      <c r="E11" s="2" t="inlineStr">
+        <is>
+          <t>Angola</t>
+        </is>
+      </c>
+      <c r="F11" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="G11" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H11" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I11" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J11" s="2" t="inlineStr">
+        <is>
+          <t>Imported cases only</t>
+        </is>
+      </c>
+      <c r="K11" s="2" t="n">
+        <v>9</v>
+      </c>
+      <c r="L11" s="2" t="n">
+        <v>5423</v>
+      </c>
+      <c r="M11" s="2" t="n"/>
+      <c r="N11" s="2" t="n"/>
+      <c r="O11" s="2" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>